<commit_message>
Added parameters to data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaunakkulkarni/PycharmProjects/untitled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2045D3F9-1093-8046-A055-35ED458E6E27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A024B1F-0AC5-B54B-93F7-F4D7A309E469}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Time(s) -Circle</t>
   </si>
@@ -29,6 +29,15 @@
   </si>
   <si>
     <t>Diameter(mm)</t>
+  </si>
+  <si>
+    <t>Spacing - 1mm</t>
+  </si>
+  <si>
+    <t>Velocity of tool - 5mm/s</t>
+  </si>
+  <si>
+    <t>Transition time- .25s</t>
   </si>
 </sst>
 </file>
@@ -2319,10 +2328,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2330,7 +2339,7 @@
     <col min="1" max="3" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2340,8 +2349,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2351,8 +2363,11 @@
       <c r="C2">
         <v>178.02192455367549</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -2362,8 +2377,11 @@
       <c r="C3">
         <v>1122.071576509747</v>
       </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>30</v>
       </c>
@@ -2374,7 +2392,7 @@
         <v>3456.8509993945609</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>40</v>
       </c>
@@ -2385,7 +2403,7 @@
         <v>7809.0861095934806</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50</v>
       </c>
@@ -2396,7 +2414,7 @@
         <v>14802.38385432504</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
@@ -2407,7 +2425,7 @@
         <v>25078.02052248118</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>70</v>
       </c>
@@ -2418,7 +2436,7 @@
         <v>39265.462876292273</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
@@ -2429,7 +2447,7 @@
         <v>57975.02181010582</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
@@ -2440,7 +2458,7 @@
         <v>81848.47214689909</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>

</xml_diff>